<commit_message>
Add the API tests for Sign Up & Assertions Enhancements
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_Login_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_Login_TestData.xlsx
@@ -3,17 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4420CDF5-6687-4C80-B0FB-C3ADE419504D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B0006-90F5-4E17-A4E5-5550FE26AB09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="29100" windowHeight="16500" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="testsheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="testsheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="API" sheetId="2" r:id="rId1"/>
+    <sheet name="GUI" sheetId="1" r:id="rId2"/>
     <sheet name="testsheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>FirstName</t>
   </si>
@@ -449,12 +453,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A63622E-CB57-6443-8D5E-E59E3D20E8B5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1155150745</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -463,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E5A4EB-72C8-0E44-91C4-D3652BB51352}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>